<commit_message>
Finished parsing the WSDL for eVASWS ORDERS
</commit_message>
<xml_diff>
--- a/order_functions/addOrderRequest.xlsx
+++ b/order_functions/addOrderRequest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Version</t>
   </si>
@@ -85,7 +85,10 @@
     <t>MediaCategory</t>
   </si>
   <si>
-    <t>ItemType</t>
+    <t>DenominationName</t>
+  </si>
+  <si>
+    <t>DenominationValue</t>
   </si>
   <si>
     <t>Count</t>
@@ -423,13 +426,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:AA1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -507,6 +510,9 @@
       </c>
       <c r="Z1" t="s">
         <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>